<commit_message>
Delete Autosaves and credit
Added commented header to main code file. Autosaves deleted.
</commit_message>
<xml_diff>
--- a/MBD Problem Solver Input.xlsx
+++ b/MBD Problem Solver Input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcorr\Documents\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcorr\Documents\GitHub\MBDS22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC8B684-625B-4924-8C3C-53A9A1E0B6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E79661-F522-4623-8991-C9A7DF786CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="432" yWindow="348" windowWidth="22608" windowHeight="8964" xr2:uid="{53A35785-85BA-4461-B078-85E0AEEDF635}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A35785-85BA-4461-B078-85E0AEEDF635}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>*ALL COLUMNS MUST HAVE AT LEAST ONE VALUE, EVEN IF IT IS A 0, OR CODE WILL NOT WORK</t>
   </si>
   <si>
-    <t xml:space="preserve">magnitude of applied force (negative if </t>
-  </si>
-  <si>
     <t>Cross-Section Type</t>
   </si>
   <si>
@@ -176,7 +173,10 @@
 Second cell: Shear Modulus value</t>
   </si>
   <si>
-    <t>Rectangular</t>
+    <t>Circular</t>
+  </si>
+  <si>
+    <t>magnitude of applied force (negative if downwards)</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -431,6 +431,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1C39F5-2643-40B0-B373-4576C6FCD449}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,28 +805,28 @@
         <v>16</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M1" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="O1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="34" t="s">
-        <v>33</v>
-      </c>
       <c r="R1" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -836,22 +837,22 @@
         <v>18</v>
       </c>
       <c r="C2" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="20">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="E2" s="19">
         <v>0</v>
       </c>
       <c r="F2" s="20">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="G2" s="21">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H2" s="19">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I2" s="22">
         <v>0</v>
@@ -860,16 +861,16 @@
         <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="2">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="M2" s="29">
-        <v>8</v>
+        <v>0.9</v>
       </c>
       <c r="N2" s="36">
-        <v>7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -890,20 +891,24 @@
         <v>19</v>
       </c>
       <c r="C3" s="10">
-        <v>8</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="11">
+        <v>-20</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.9</v>
+      </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10"/>
       <c r="L3" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3" s="28">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="2">
@@ -917,7 +922,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="10"/>
@@ -928,7 +933,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="11"/>
       <c r="J4" s="10"/>
-      <c r="M4" s="25"/>
+      <c r="M4" s="37"/>
       <c r="O4" s="2"/>
       <c r="P4" s="28"/>
     </row>
@@ -974,7 +979,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
@@ -995,28 +1000,28 @@
         <v>4</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="M10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now plots a y=0
Slightly improved plotting (we can definitely make it neater with some axis labels and a legend and whatnot).
</commit_message>
<xml_diff>
--- a/MBD Problem Solver Input.xlsx
+++ b/MBD Problem Solver Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcorr\Documents\GitHub\MBDS22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E79661-F522-4623-8991-C9A7DF786CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BACAE1-DE24-4185-BB7D-80E1749E3A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A35785-85BA-4461-B078-85E0AEEDF635}"/>
   </bookViews>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1C39F5-2643-40B0-B373-4576C6FCD449}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,7 +916,7 @@
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="25">
-        <v>16</v>
+        <v>1.5</v>
       </c>
       <c r="R3" s="31">
         <v>20000</v>

</xml_diff>

<commit_message>
Torsion Calculations care about your feelings now
Only sums torsions up to the point on the beam you want the stress at. Same for angle of twist. (Before it would always use the torsion at the very end of the beam).
</commit_message>
<xml_diff>
--- a/MBD Problem Solver Input.xlsx
+++ b/MBD Problem Solver Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcorr\Documents\GitHub\MBDS22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BACAE1-DE24-4185-BB7D-80E1749E3A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258F13E9-1803-420D-B9E7-C2A98F79EEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A35785-85BA-4461-B078-85E0AEEDF635}"/>
   </bookViews>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1C39F5-2643-40B0-B373-4576C6FCD449}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,10 +837,10 @@
         <v>18</v>
       </c>
       <c r="C2" s="19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D2" s="20">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="E2" s="19">
         <v>0</v>
@@ -864,22 +864,22 @@
         <v>43</v>
       </c>
       <c r="L2" s="2">
-        <v>0.04</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="M2" s="29">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="N2" s="36">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>0</v>
+        <v>3.18</v>
       </c>
       <c r="P2" s="32">
         <v>0</v>
       </c>
       <c r="Q2" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="33">
         <v>10000</v>
@@ -891,13 +891,13 @@
         <v>19</v>
       </c>
       <c r="C3" s="10">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="D3" s="11">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="E3" s="10">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
@@ -908,15 +908,17 @@
         <v>0</v>
       </c>
       <c r="M3" s="28">
-        <v>0.04</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2"/>
+        <v>6.37</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
       <c r="Q3" s="25">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="R3" s="31">
         <v>20000</v>
@@ -934,8 +936,12 @@
       <c r="I4" s="11"/>
       <c r="J4" s="10"/>
       <c r="M4" s="37"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="28"/>
+      <c r="O4" s="2">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="P4" s="28">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>

</xml_diff>

<commit_message>
Update MBD Problem Solver Input.xlsx
working test case for singular axial torque causing torsion (both angle of twist and torsional shear stress work)
</commit_message>
<xml_diff>
--- a/MBD Problem Solver Input.xlsx
+++ b/MBD Problem Solver Input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcorr\Documents\GitHub\MBDS22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenr\Documents\GitHub\MBDS22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258F13E9-1803-420D-B9E7-C2A98F79EEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59F0D52-BEEF-436E-8BE7-584B7A4F9F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A35785-85BA-4461-B078-85E0AEEDF635}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53A35785-85BA-4461-B078-85E0AEEDF635}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,14 +169,14 @@
 First cell: target distance from left end of beam</t>
   </si>
   <si>
-    <t>First cell: Young's Modulus value
-Second cell: Shear Modulus value</t>
-  </si>
-  <si>
     <t>Circular</t>
   </si>
   <si>
     <t>magnitude of applied force (negative if downwards)</t>
+  </si>
+  <si>
+    <t>First cell: Young's Modulus value, E
+Second cell: Shear Modulus value, G</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,10 +861,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L2" s="2">
-        <v>1.2500000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M2" s="29">
         <v>0</v>
@@ -873,13 +873,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>3.18</v>
+        <v>50</v>
       </c>
       <c r="P2" s="32">
         <v>0</v>
       </c>
       <c r="Q2" s="29">
-        <v>1</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R2" s="33">
         <v>10000</v>
@@ -904,24 +904,19 @@
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="10"/>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
+      <c r="L3" s="3"/>
       <c r="M3" s="28">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="2">
-        <v>6.37</v>
-      </c>
-      <c r="P3" s="2">
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="25">
         <v>1</v>
       </c>
-      <c r="Q3" s="25">
-        <v>2</v>
-      </c>
       <c r="R3" s="31">
-        <v>20000</v>
+        <f>27*10^9</f>
+        <v>27000000000</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -936,12 +931,8 @@
       <c r="I4" s="11"/>
       <c r="J4" s="10"/>
       <c r="M4" s="37"/>
-      <c r="O4" s="2">
-        <v>9.5500000000000007</v>
-      </c>
-      <c r="P4" s="28">
-        <v>2</v>
-      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
@@ -985,7 +976,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
@@ -1027,7 +1018,7 @@
         <v>38</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>